<commit_message>
Updated database for the life cycle knowledge base part.
</commit_message>
<xml_diff>
--- a/backend/api/kb/lifecycle-to-plant.xlsx
+++ b/backend/api/kb/lifecycle-to-plant.xlsx
@@ -411,7 +411,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -423,6 +423,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -449,9 +455,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -756,7 +763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B116"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D111" sqref="D111"/>
     </sheetView>
   </sheetViews>
@@ -1704,7 +1711,7 @@
   <dimension ref="B2:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1745,7 +1752,7 @@
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Can now push life cycle data, and also improved algorithms.
</commit_message>
<xml_diff>
--- a/backend/api/kb/lifecycle-to-plant.xlsx
+++ b/backend/api/kb/lifecycle-to-plant.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="KB" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="133">
   <si>
     <t>plant_type</t>
   </si>
@@ -405,6 +405,15 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/Perennial_plant</t>
+  </si>
+  <si>
+    <t>For row 117 (Cactus)</t>
+  </si>
+  <si>
+    <t>https://www.hunker.com/13427982/are-succulents-perennials</t>
+  </si>
+  <si>
+    <t>Cactus</t>
   </si>
 </sst>
 </file>
@@ -761,10 +770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B116"/>
+  <dimension ref="A1:B117"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D111" sqref="D111"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1701,6 +1710,14 @@
         <v>38</v>
       </c>
     </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>132</v>
+      </c>
+      <c r="B117" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1708,10 +1725,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B22"/>
+  <dimension ref="B2:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1791,12 +1808,23 @@
         <v>129</v>
       </c>
     </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B13" r:id="rId1"/>
     <hyperlink ref="B16" r:id="rId2"/>
     <hyperlink ref="B19" r:id="rId3"/>
     <hyperlink ref="B22" r:id="rId4"/>
+    <hyperlink ref="B25" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>